<commit_message>
Updated with runtime measurement
</commit_message>
<xml_diff>
--- a/Sample Datasets/appointment sample data.xlsx
+++ b/Sample Datasets/appointment sample data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive - National University of Singapore\NUS\Internships\GovTech\Project - Network Graphs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Dev\GovTech Projects\Graphdb_govtech\Sample Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{992F817E-64D5-4A4A-B69D-F5A57217C2C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00E1A4F2-E865-4F59-AC4B-5E244655A006}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B33805-6150-426D-8131-0E0B1EB80D77}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{84258B7E-50EB-474A-98D6-95790CA7AD9F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Entity UEN</t>
   </si>
@@ -70,6 +70,30 @@
   </si>
   <si>
     <t>app10</t>
+  </si>
+  <si>
+    <t>Appointment Name</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>HR Manager</t>
+  </si>
+  <si>
+    <t>Tech Lead</t>
+  </si>
+  <si>
+    <t>Finance Manager</t>
+  </si>
+  <si>
+    <t>Deputy Director</t>
+  </si>
+  <si>
+    <t>en5</t>
+  </si>
+  <si>
+    <t>app5</t>
   </si>
 </sst>
 </file>
@@ -431,64 +455,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACC480A-28CB-4987-B4D3-22BC260731D4}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -498,6 +552,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009D477D0D98DC664BA91CBEC9A9ACF2B9" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a1959c30aeb4e0277fb9d7ed33a24d56">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1c5a4cdb-cf1f-4189-9f9d-57300d5db6d2" xmlns:ns4="3ce8712f-b9ab-41c9-b70b-997cb8aa2f45" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ae7f75cefe26a8647b7bff25f567909" ns3:_="" ns4:_="">
     <xsd:import namespace="1c5a4cdb-cf1f-4189-9f9d-57300d5db6d2"/>
@@ -706,15 +769,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -722,6 +776,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F394FE0A-15F5-4C85-A8D8-48A6B54D2040}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CE5005D-2921-4465-9702-03D512229205}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -740,14 +802,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F394FE0A-15F5-4C85-A8D8-48A6B54D2040}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EBD8343-023D-40A9-B7C8-CF2242DA836E}">
   <ds:schemaRefs>

</xml_diff>